<commit_message>
Gsheets connection indicator done
</commit_message>
<xml_diff>
--- a/logs/post_logs.xlsx
+++ b/logs/post_logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3836,6 +3836,1921 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr"/>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="inlineStr"/>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="n">
+        <v>1</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>21:00:00</t>
+        </is>
+      </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr"/>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="n">
+        <v>2</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>21:30:00</t>
+        </is>
+      </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr"/>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="n">
+        <v>3</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr"/>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>21:00:00</t>
+        </is>
+      </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr"/>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr"/>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="inlineStr"/>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="n">
+        <v>2</v>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>21:30:00</t>
+        </is>
+      </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr"/>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr"/>
+      <c r="D62" t="inlineStr"/>
+      <c r="E62" t="inlineStr"/>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="n">
+        <v>3</v>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr"/>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="inlineStr"/>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="n">
+        <v>1</v>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>21:00:00</t>
+        </is>
+      </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr"/>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="inlineStr"/>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="n">
+        <v>2</v>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>21:30:00</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr"/>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="n">
+        <v>3</v>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr"/>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>21:00:00</t>
+        </is>
+      </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr"/>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="n">
+        <v>2</v>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>21:30:00</t>
+        </is>
+      </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr"/>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="n">
+        <v>3</v>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr"/>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="n">
+        <v>1</v>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr"/>
+      <c r="B70" t="inlineStr"/>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="n">
+        <v>2</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>22:30:00</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr"/>
+      <c r="B71" t="inlineStr"/>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="n">
+        <v>3</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr"/>
+      <c r="B72" t="inlineStr"/>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="n">
+        <v>1</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr"/>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="n">
+        <v>2</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>22:30:00</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr"/>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="n">
+        <v>3</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr"/>
+      <c r="B75" t="inlineStr"/>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr"/>
+      <c r="B76" t="inlineStr"/>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="n">
+        <v>2</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>22:30:00</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr"/>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="n">
+        <v>3</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr"/>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="n">
+        <v>1</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr"/>
+      <c r="B79" t="inlineStr"/>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="n">
+        <v>2</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>22:30:00</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr"/>
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="n">
+        <v>3</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr"/>
+      <c r="B81" t="inlineStr"/>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>22:00:00</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr"/>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="n">
+        <v>2</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>22:30:00</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr"/>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="n">
+        <v>3</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>2025-08-31</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>23:00:00</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr"/>
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="n">
+        <v>1</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>18:10:00</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image)</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr"/>
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="n">
+        <v>1</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>18:10:00</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr"/>
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="n">
+        <v>2</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>21:05:00</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image+Caption)</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr"/>
+      <c r="B87" t="inlineStr"/>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="n">
+        <v>2</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>21:05:00</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr"/>
+      <c r="B88" t="inlineStr"/>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="n">
+        <v>3</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>21:10:00</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image+Caption)</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr"/>
+      <c r="B89" t="inlineStr"/>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="n">
+        <v>3</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>2025-09-02</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>21:10:00</t>
+        </is>
+      </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr"/>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="n">
+        <v>1</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>18:00:00</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image)</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr"/>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="n">
+        <v>1</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>18:00:00</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr"/>
+      <c r="B92" t="inlineStr"/>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="n">
+        <v>2</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>21:05:00</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr"/>
+      <c r="B93" t="inlineStr"/>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="inlineStr"/>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="n">
+        <v>3</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>21:10:00</t>
+        </is>
+      </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr"/>
+      <c r="B94" t="inlineStr"/>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="n">
+        <v>1</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>18:10:00</t>
+        </is>
+      </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image only)</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr"/>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr"/>
+      <c r="B95" t="inlineStr"/>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="n">
+        <v>1</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>18:10:00</t>
+        </is>
+      </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr"/>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="n">
+        <v>2</v>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>21:05:00</t>
+        </is>
+      </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr"/>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="n">
+        <v>3</v>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>21:10:00</t>
+        </is>
+      </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr"/>
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr"/>
+      <c r="D98" t="inlineStr"/>
+      <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="n">
+        <v>1</v>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>18:00:00</t>
+        </is>
+      </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image only)</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr"/>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr"/>
+      <c r="B99" t="inlineStr"/>
+      <c r="C99" t="inlineStr"/>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="n">
+        <v>1</v>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>Kid's Carnival</t>
+        </is>
+      </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>18:00:00</t>
+        </is>
+      </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+🔥 **DEMO DEALS OF THE DAY** 🔥
+💥 Price Crash Store
+⚡️ Up to 5% off
+👉🏻 amzaff.in/l3swo0g
+🌟 Kid's Carnival
+📣 Sale live till 28th July
+👉🏻 amzaff.in/jrtPYsT
+🧸 Toy's Fiesta
+⚡️ Up to 70% off...</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr"/>
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr"/>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="n">
+        <v>2</v>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>Daily Essentials</t>
+        </is>
+      </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>10:05:00</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💧 **DEMO Essentials for Skin, Hair &amp; Fragrance** 💧
+💥 Maximise earnings with Beauty commissions – Now increased to 10%
+🌿 Mamaearth Rice Oil-Free Face Moisturizer for Oily Skin
+⚡️ 80g...</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr"/>
+      <c r="B101" t="inlineStr"/>
+      <c r="C101" t="inlineStr"/>
+      <c r="D101" t="inlineStr"/>
+      <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="n">
+        <v>3</v>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>Laptops</t>
+        </is>
+      </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>2025-09-03</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>10:10:00</t>
+        </is>
+      </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>DEMO_POST
+💻 **DEMO Level Gaming Laptops**
+⚡️ Up to 45% off
+👉🏻 amzaff.in/FeVABNi
+🔥 Gaming Laptops Under ₹80,000 🔥
+💻 ASUS TUF A15 GAMING
+⚡️ ~~₹83,990~~ | ₹63,990
+⚡️ Effective price ₹56,490
+👉🏻 amzaff...</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new commit link clicks
</commit_message>
<xml_diff>
--- a/logs/post_logs.xlsx
+++ b/logs/post_logs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L101"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -515,6 +515,11 @@
           <t>Message</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Channel</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -572,6 +577,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -634,6 +640,7 @@
       <c r="J3" t="inlineStr"/>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -691,6 +698,7 @@
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -758,6 +766,7 @@
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -815,6 +824,7 @@
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -875,6 +885,7 @@
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -958,6 +969,7 @@
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1024,6 +1036,7 @@
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1083,6 +1096,7 @@
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1166,6 +1180,7 @@
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1223,6 +1238,7 @@
       <c r="J12" t="inlineStr"/>
       <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1288,6 +1304,7 @@
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr"/>
       <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1342,6 +1359,7 @@
       <c r="J14" t="inlineStr"/>
       <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1401,6 +1419,7 @@
       <c r="J15" t="inlineStr"/>
       <c r="K15" t="inlineStr"/>
       <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1460,6 +1479,7 @@
       <c r="J16" t="inlineStr"/>
       <c r="K16" t="inlineStr"/>
       <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1526,6 +1546,7 @@
       <c r="J17" t="inlineStr"/>
       <c r="K17" t="inlineStr"/>
       <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1591,6 +1612,7 @@
       <c r="J18" t="inlineStr"/>
       <c r="K18" t="inlineStr"/>
       <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1650,6 +1672,7 @@
       <c r="J19" t="inlineStr"/>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1712,6 +1735,7 @@
       <c r="J20" t="inlineStr"/>
       <c r="K20" t="inlineStr"/>
       <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -1767,6 +1791,7 @@
 👉🏻 amzaff.in/dvgN1JH</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -1820,6 +1845,7 @@
 👉🏻 amzaff.in/IQsEdXX</t>
         </is>
       </c>
+      <c r="M22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -1884,6 +1910,7 @@
 👉🏻 amzaff.in/R4IV7C8</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -1944,6 +1971,7 @@
 #3 Including bank coupon offer</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -2001,6 +2029,7 @@
 👉🏻 amzaff.in/Z2bNfA5</t>
         </is>
       </c>
+      <c r="M25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -2064,6 +2093,7 @@
 👉🏻 amzaff.in/srnrpxV</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -2121,6 +2151,7 @@
 👉🏻 amzaff.in/4BT4gvh</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
@@ -2183,6 +2214,7 @@
 👉🏻 amzaff.in/FfxM93V</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
@@ -2240,6 +2272,7 @@
 👉🏻 amzaff.in/s4QD0BJ</t>
         </is>
       </c>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
@@ -2305,6 +2338,7 @@
 👉🏻 amzaff.in/XhZb3MA</t>
         </is>
       </c>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -2362,6 +2396,7 @@
 👉🏻 amzaff.in/9Y8v39c</t>
         </is>
       </c>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -2426,6 +2461,7 @@
 👉🏻 amzaff.in/JMe8Xdr</t>
         </is>
       </c>
+      <c r="M32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
@@ -2491,6 +2527,7 @@
 👉🏻 amzaff.in/1bEQTPW</t>
         </is>
       </c>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -2551,6 +2588,7 @@
 👉🏻 amzaff.in/jZzk4Ks</t>
         </is>
       </c>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -2613,6 +2651,7 @@
 👉🏻 amzaff.in/B30aWTr</t>
         </is>
       </c>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -2672,6 +2711,7 @@
 👉🏻 amzaff.in/1QS8Ixk</t>
         </is>
       </c>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -2734,6 +2774,7 @@
 👉🏻 amzaff.in/OUxqJDH</t>
         </is>
       </c>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
@@ -2792,6 +2833,7 @@
 👉🏻 amzaff.in/V2sI4x5</t>
         </is>
       </c>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr"/>
@@ -2849,6 +2891,7 @@
 👉🏻 amzaff.in/Nj7ktWN</t>
         </is>
       </c>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -2908,6 +2951,7 @@
 👉🏻 amzaff.in/36KEtuX</t>
         </is>
       </c>
+      <c r="M40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
@@ -2968,6 +3012,7 @@
 👉🏻 amzaff.in/mx4k7sB</t>
         </is>
       </c>
+      <c r="M41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
@@ -3027,6 +3072,7 @@
 👉🏻 amzaff.in/kEbYPKD</t>
         </is>
       </c>
+      <c r="M42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -3087,6 +3133,7 @@
 👉🏻 amzaff.in/PtQuEV0</t>
         </is>
       </c>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -3147,6 +3194,7 @@
 👉🏻 amzaff.in/dqc4h6R</t>
         </is>
       </c>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
@@ -3202,6 +3250,7 @@
 👉🏻 amzaff.in/dvgN1JH</t>
         </is>
       </c>
+      <c r="M45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -3255,6 +3304,7 @@
 👉🏻 amzaff.in/IQsEdXX</t>
         </is>
       </c>
+      <c r="M46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -3319,6 +3369,7 @@
 👉🏻 amzaff.in/R4IV7C8</t>
         </is>
       </c>
+      <c r="M47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
@@ -3374,6 +3425,7 @@
 👉🏻 amzaff.in/dvgN1JH</t>
         </is>
       </c>
+      <c r="M48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
@@ -3427,6 +3479,7 @@
 👉🏻 amzaff.in/IQsEdXX</t>
         </is>
       </c>
+      <c r="M49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -3491,6 +3544,7 @@
 👉🏻 amzaff.in/R4IV7C8</t>
         </is>
       </c>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -3546,6 +3600,7 @@
 👉🏻 amzaff.in/dvgN1JH</t>
         </is>
       </c>
+      <c r="M51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr"/>
@@ -3599,6 +3654,7 @@
 👉🏻 amzaff.in/IQsEdXX</t>
         </is>
       </c>
+      <c r="M52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr"/>
@@ -3663,6 +3719,7 @@
 👉🏻 amzaff.in/R4IV7C8</t>
         </is>
       </c>
+      <c r="M53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr"/>
@@ -3718,6 +3775,7 @@
 👉🏻 amzaff.in/dvgN1JH</t>
         </is>
       </c>
+      <c r="M54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
@@ -3771,6 +3829,7 @@
 👉🏻 amzaff.in/IQsEdXX</t>
         </is>
       </c>
+      <c r="M55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr"/>
@@ -3835,6 +3894,7 @@
 👉🏻 amzaff.in/R4IV7C8</t>
         </is>
       </c>
+      <c r="M56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
@@ -3880,6 +3940,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr"/>
@@ -3920,6 +3981,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr"/>
@@ -3964,6 +4026,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr"/>
@@ -4009,6 +4072,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr"/>
@@ -4049,6 +4113,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr"/>
@@ -4093,6 +4158,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -4138,6 +4204,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr"/>
@@ -4178,6 +4245,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr"/>
@@ -4222,6 +4290,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr"/>
@@ -4267,6 +4336,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr"/>
@@ -4307,6 +4377,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr"/>
@@ -4351,6 +4422,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr"/>
@@ -4396,6 +4468,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr"/>
@@ -4436,6 +4509,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr"/>
@@ -4480,6 +4554,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr"/>
@@ -4525,6 +4600,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr"/>
@@ -4565,6 +4641,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr"/>
@@ -4609,6 +4686,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
@@ -4654,6 +4732,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr"/>
@@ -4694,6 +4773,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr"/>
@@ -4738,6 +4818,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr"/>
@@ -4783,6 +4864,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
@@ -4823,6 +4905,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>
@@ -4867,6 +4950,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr"/>
@@ -4912,6 +4996,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr"/>
@@ -4952,6 +5037,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
@@ -4996,6 +5082,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr"/>
@@ -5041,6 +5128,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr"/>
@@ -5086,6 +5174,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr"/>
@@ -5126,6 +5215,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
@@ -5166,6 +5256,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr"/>
@@ -5210,6 +5301,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -5254,6 +5346,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr"/>
@@ -5299,6 +5392,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
@@ -5344,6 +5438,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr"/>
@@ -5384,6 +5479,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr"/>
@@ -5428,6 +5524,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr"/>
@@ -5460,6 +5557,7 @@
         </is>
       </c>
       <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
@@ -5505,6 +5603,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
@@ -5545,6 +5644,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr"/>
@@ -5589,6 +5689,7 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr"/>
@@ -5621,6 +5722,7 @@
         </is>
       </c>
       <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
@@ -5666,6 +5768,7 @@
 ⚡️ Up to 70% off...</t>
         </is>
       </c>
+      <c r="M99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>
@@ -5706,6 +5809,7 @@
 ⚡️ 80g...</t>
         </is>
       </c>
+      <c r="M100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr"/>
@@ -5750,6 +5854,220 @@
 👉🏻 amzaff...</t>
         </is>
       </c>
+      <c r="M101" t="inlineStr"/>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr"/>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="n">
+        <v>15</v>
+      </c>
+      <c r="H102" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>18:05:00</t>
+        </is>
+      </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>✅ Scheduled (Image only)</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr">
+        <is>
+          <t>amazonindiaassociates</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr"/>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="n">
+        <v>15</v>
+      </c>
+      <c r="H103" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>18:05:00</t>
+        </is>
+      </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>⚠️ No Content</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>No text or image provided</t>
+        </is>
+      </c>
+      <c r="M103" t="inlineStr">
+        <is>
+          <t>amazonindiaassociates</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr"/>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="n">
+        <v>15</v>
+      </c>
+      <c r="H104" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>18:05:00</t>
+        </is>
+      </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>🎧 **Wireless &amp; Headphones**
+⚡ Up to 75% off
+🎉 **Great Indian Festival 📣  Live Now**
+🌟  **Great Deals | No Cost EMI | Exchange Offer**
+- 10% Instant Discount upto ₹1.4Lakh. Offer resets on every...</t>
+        </is>
+      </c>
+      <c r="M104" t="inlineStr">
+        <is>
+          <t>amazonindiaassociates</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr"/>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="n">
+        <v>15</v>
+      </c>
+      <c r="H105" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>18:05:00</t>
+        </is>
+      </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>❌ Failed: cannot access local variable 'error_msg' where it is not associated with a value</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>🎧 **Wireless &amp; Headphones**
+⚡ Up to 75% off
+🎉 **Great Indian Festival 📣  Live Now**
+🌟  **Great Deals | No Cost EMI | Exchange Offer**
+- 10% Instant Discount upto ₹1.4Lakh. Offer resets on every...</t>
+        </is>
+      </c>
+      <c r="M105" t="inlineStr">
+        <is>
+          <t>amazonindiaassociates</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr"/>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="n">
+        <v>16</v>
+      </c>
+      <c r="H106" t="inlineStr">
+        <is>
+          <t>Uncategorized</t>
+        </is>
+      </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>2025-10-01</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>18:35:00</t>
+        </is>
+      </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>✅ Scheduled</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>🔥 **Samsung Washing Machines**
+⚡ Up to 40% off
+🎉 **Great Indian Festival 📣  Live Now**
+🌟  **Great Deals | No Cost EMI | Exchange Offer**
+- 10% Instant Discount upto ₹1.4Lakh. Offer resets on...</t>
+        </is>
+      </c>
+      <c r="M106" t="inlineStr">
+        <is>
+          <t>amazonindiaassociates</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>